<commit_message>
sheet names in xlsx
</commit_message>
<xml_diff>
--- a/excel_input_files/Test_input_Condition1Neg.xlsx
+++ b/excel_input_files/Test_input_Condition1Neg.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Desktop\Glasgow\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simon/git/lipid_prototype/excel_input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C276F3E7-3F14-4C28-8DBA-69510EBC15BC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7021200-0A4D-BE4F-993A-6EFD7E349E60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{59EBD085-9D3B-4EB6-B56D-6019178B6EC5}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{59EBD085-9D3B-4EB6-B56D-6019178B6EC5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
+    <sheet name="lipids" sheetId="3" r:id="rId1"/>
+    <sheet name="files" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="87">
   <si>
     <t>Name</t>
   </si>
@@ -281,9 +281,6 @@
   </si>
   <si>
     <t>24_pp_d20_neg_1</t>
-  </si>
-  <si>
-    <t>Theoretical mass</t>
   </si>
   <si>
     <t>PC(38:2)</t>
@@ -721,21 +718,21 @@
   <dimension ref="A1:M40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="19.77734375" customWidth="1"/>
-    <col min="5" max="5" width="24.77734375" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" customWidth="1"/>
+    <col min="5" max="5" width="24.83203125" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -760,11 +757,9 @@
       <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>57</v>
       </c>
@@ -787,11 +782,8 @@
         <v>20</v>
       </c>
       <c r="H2" s="3"/>
-      <c r="J2">
-        <v>759.57835399999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -814,11 +806,8 @@
         <v>20</v>
       </c>
       <c r="H3" s="3"/>
-      <c r="J3">
-        <v>757.56270400000005</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>44</v>
       </c>
@@ -841,11 +830,8 @@
         <v>20</v>
       </c>
       <c r="H4" s="3"/>
-      <c r="J4">
-        <v>759.57835399999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>45</v>
       </c>
@@ -868,12 +854,9 @@
         <v>20</v>
       </c>
       <c r="H5" s="3"/>
-      <c r="J5">
-        <v>785.59400400000004</v>
-      </c>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>58</v>
       </c>
@@ -896,12 +879,9 @@
         <v>20</v>
       </c>
       <c r="H6" s="3"/>
-      <c r="J6">
-        <v>761.59400400000004</v>
-      </c>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>46</v>
       </c>
@@ -924,13 +904,10 @@
         <v>20</v>
       </c>
       <c r="H7" s="3"/>
-      <c r="J7">
-        <v>757.56270400000005</v>
-      </c>
       <c r="L7" s="2"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>47</v>
       </c>
@@ -953,12 +930,9 @@
         <v>20</v>
       </c>
       <c r="H8" s="3"/>
-      <c r="J8">
-        <v>787.60965399999998</v>
-      </c>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>48</v>
       </c>
@@ -981,12 +955,9 @@
         <v>20</v>
       </c>
       <c r="H9" s="3"/>
-      <c r="J9">
-        <v>771.61473899999999</v>
-      </c>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>49</v>
       </c>
@@ -1009,12 +980,9 @@
         <v>20</v>
       </c>
       <c r="H10" s="3"/>
-      <c r="J10">
-        <v>764.69293000000005</v>
-      </c>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>50</v>
       </c>
@@ -1038,12 +1006,10 @@
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="9"/>
-      <c r="J11" s="9">
-        <v>761.59400400000004</v>
-      </c>
+      <c r="J11" s="9"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>51</v>
       </c>
@@ -1067,17 +1033,15 @@
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="9"/>
-      <c r="J12" s="9">
-        <v>783.57835399999999</v>
-      </c>
+      <c r="J12" s="9"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>80</v>
@@ -1096,14 +1060,12 @@
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="9"/>
-      <c r="J13" s="9">
-        <v>773.59400400000004</v>
-      </c>
+      <c r="J13" s="9"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>20</v>
@@ -1125,12 +1087,10 @@
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="9"/>
-      <c r="J14" s="9">
-        <v>813.62530400000003</v>
-      </c>
+      <c r="J14" s="9"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>52</v>
       </c>
@@ -1154,12 +1114,10 @@
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="9"/>
-      <c r="J15" s="9">
-        <v>789.62530400000003</v>
-      </c>
+      <c r="J15" s="9"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>53</v>
       </c>
@@ -1183,12 +1141,10 @@
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="9"/>
-      <c r="J16" s="9">
-        <v>719.547054</v>
-      </c>
+      <c r="J16" s="9"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>54</v>
       </c>
@@ -1212,12 +1168,10 @@
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="9"/>
-      <c r="J17" s="9">
-        <v>731.547054</v>
-      </c>
+      <c r="J17" s="9"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>55</v>
       </c>
@@ -1241,12 +1195,10 @@
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="9"/>
-      <c r="J18" s="9">
-        <v>731.583439</v>
-      </c>
+      <c r="J18" s="9"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>60</v>
       </c>
@@ -1270,12 +1222,10 @@
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="9"/>
-      <c r="J19" s="9">
-        <v>729.53140299999995</v>
-      </c>
+      <c r="J19" s="9"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>56</v>
       </c>
@@ -1299,12 +1249,10 @@
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="9"/>
-      <c r="J20" s="9">
-        <v>743.547054</v>
-      </c>
+      <c r="J20" s="9"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
@@ -1328,12 +1276,10 @@
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="9"/>
-      <c r="J21" s="9">
-        <v>809.59400400000004</v>
-      </c>
+      <c r="J21" s="9"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>29</v>
       </c>
@@ -1357,12 +1303,10 @@
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="9"/>
-      <c r="J22" s="9">
-        <v>833.59400400000004</v>
-      </c>
+      <c r="J22" s="9"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>31</v>
       </c>
@@ -1386,12 +1330,10 @@
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="9"/>
-      <c r="J23" s="9">
-        <v>733.56270400000005</v>
-      </c>
+      <c r="J23" s="9"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>33</v>
       </c>
@@ -1415,12 +1357,10 @@
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="9"/>
-      <c r="J24" s="9">
-        <v>549.37998800000003</v>
-      </c>
+      <c r="J24" s="9"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>35</v>
       </c>
@@ -1444,12 +1384,10 @@
       </c>
       <c r="H25" s="3"/>
       <c r="I25" s="9"/>
-      <c r="J25" s="9">
-        <v>479.301738</v>
-      </c>
+      <c r="J25" s="9"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>37</v>
       </c>
@@ -1473,12 +1411,10 @@
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="9"/>
-      <c r="J26" s="9">
-        <v>501.28608800000001</v>
-      </c>
+      <c r="J26" s="9"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>39</v>
       </c>
@@ -1502,12 +1438,10 @@
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="9"/>
-      <c r="J27" s="9">
-        <v>815.64095399999997</v>
-      </c>
+      <c r="J27" s="9"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>40</v>
       </c>
@@ -1531,12 +1465,10 @@
       </c>
       <c r="H28" s="3"/>
       <c r="I28" s="9"/>
-      <c r="J28" s="9">
-        <v>813.62530400000003</v>
-      </c>
+      <c r="J28" s="9"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>41</v>
       </c>
@@ -1560,12 +1492,10 @@
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="9"/>
-      <c r="J29" s="9">
-        <v>833.59400400000004</v>
-      </c>
+      <c r="J29" s="9"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>43</v>
       </c>
@@ -1589,12 +1519,10 @@
       </c>
       <c r="H30" s="3"/>
       <c r="I30" s="9"/>
-      <c r="J30" s="9">
-        <v>793.59908900000005</v>
-      </c>
+      <c r="J30" s="9"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>61</v>
       </c>
@@ -1618,12 +1546,10 @@
       </c>
       <c r="H31" s="3"/>
       <c r="I31" s="9"/>
-      <c r="J31" s="9">
-        <v>304.24077899999997</v>
-      </c>
+      <c r="J31" s="9"/>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>62</v>
       </c>
@@ -1647,11 +1573,9 @@
       </c>
       <c r="H32" s="3"/>
       <c r="I32" s="9"/>
-      <c r="J32" s="9">
-        <v>304.24077899999997</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J32" s="9"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>63</v>
       </c>
@@ -1675,11 +1599,9 @@
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="9"/>
-      <c r="J33" s="9">
-        <v>479.301738</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J33" s="9"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>64</v>
       </c>
@@ -1703,11 +1625,9 @@
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="9"/>
-      <c r="J34" s="9">
-        <v>501.28608800000001</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J34" s="9"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>75</v>
       </c>
@@ -1731,11 +1651,9 @@
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="9"/>
-      <c r="J35" s="9">
-        <v>723.52083900000002</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J35" s="9"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
         <v>65</v>
       </c>
@@ -1759,11 +1677,9 @@
       </c>
       <c r="H36" s="3"/>
       <c r="I36" s="9"/>
-      <c r="J36" s="9">
-        <v>739.51575300000002</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J36" s="9"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>66</v>
       </c>
@@ -1787,16 +1703,14 @@
       </c>
       <c r="H37" s="3"/>
       <c r="I37" s="9"/>
-      <c r="J37" s="9">
-        <v>751.55213900000001</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J37" s="9"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
         <v>67</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>80</v>
@@ -1815,13 +1729,11 @@
       </c>
       <c r="H38" s="3"/>
       <c r="I38" s="9"/>
-      <c r="J38" s="9">
-        <v>765.53140299999995</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J38" s="9"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B39" s="12" t="s">
         <v>79</v>
@@ -1843,11 +1755,9 @@
       </c>
       <c r="H39" s="3"/>
       <c r="I39" s="9"/>
-      <c r="J39" s="9">
-        <v>783.541968</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J39" s="9"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1872,12 +1782,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1885,7 +1795,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -1893,7 +1803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -1901,7 +1811,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>82</v>
       </c>
@@ -1909,7 +1819,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>70</v>
       </c>
@@ -1917,7 +1827,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>72</v>
       </c>
@@ -1925,7 +1835,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -1933,7 +1843,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
started changing parse xlsx
</commit_message>
<xml_diff>
--- a/excel_input_files/Test_input_Condition1Neg.xlsx
+++ b/excel_input_files/Test_input_Condition1Neg.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simon/git/lipid_prototype/excel_input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720F52E9-B013-CB49-9C92-5D23CE7F9CA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CDE289-703A-6849-94B1-DD4B38E091DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" activeTab="1" xr2:uid="{59EBD085-9D3B-4EB6-B56D-6019178B6EC5}"/>
+    <workbookView xWindow="30980" yWindow="1480" windowWidth="23260" windowHeight="12580" activeTab="2" xr2:uid="{59EBD085-9D3B-4EB6-B56D-6019178B6EC5}"/>
   </bookViews>
   <sheets>
     <sheet name="lipids" sheetId="3" r:id="rId1"/>
     <sheet name="files" sheetId="4" r:id="rId2"/>
+    <sheet name="parameters" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="89">
   <si>
     <t>Name</t>
   </si>
@@ -293,6 +294,12 @@
   </si>
   <si>
     <t>PE(38:4p(12OH[S]))</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>value</t>
   </si>
 </sst>
 </file>
@@ -1778,7 +1785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6D3203F-BC1B-7745-B9F8-C5C7D6E73FC7}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1854,4 +1861,27 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE9C0786-739C-D54D-82F4-D057694BAA36}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
better parameterisation for test
</commit_message>
<xml_diff>
--- a/excel_input_files/Test_input_Condition1Neg.xlsx
+++ b/excel_input_files/Test_input_Condition1Neg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simon/git/lipid_prototype/excel_input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CDE289-703A-6849-94B1-DD4B38E091DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4B91D7-8F10-4245-90E8-B6EBC0322E2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30980" yWindow="1480" windowWidth="23260" windowHeight="12580" activeTab="2" xr2:uid="{59EBD085-9D3B-4EB6-B56D-6019178B6EC5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="90">
   <si>
     <t>Name</t>
   </si>
@@ -300,6 +300,9 @@
   </si>
   <si>
     <t>value</t>
+  </si>
+  <si>
+    <t>max_iso_n</t>
   </si>
 </sst>
 </file>
@@ -1865,10 +1868,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE9C0786-739C-D54D-82F4-D057694BAA36}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1881,6 +1884,14 @@
         <v>88</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>